<commit_message>
Updated who has which items
</commit_message>
<xml_diff>
--- a/UVM-NRT-RoS/equipment-records/CIROH_Items_Comprehensive_List.xlsx
+++ b/UVM-NRT-RoS/equipment-records/CIROH_Items_Comprehensive_List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f59c65449ee1dfc/Documents/UVM/2024-2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CIROH_Repository\CIROH-NextGen-SMS-UVM\UVM-NRT-RoS\equipment-records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{7FC9091D-619A-415D-A7BC-F586D5289D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16FE9789-68AE-4990-8767-25E80252BF1D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3730C9DF-AD33-4914-9F73-C6D1EEB69BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{E103461D-B812-4EE3-B8B5-011B2C0D6DE5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
   <si>
     <t>Item</t>
   </si>
@@ -287,6 +287,30 @@
   </si>
   <si>
     <t>Soheyl</t>
+  </si>
+  <si>
+    <t>Microphone Setup</t>
+  </si>
+  <si>
+    <t>Soheyl + Casey</t>
+  </si>
+  <si>
+    <t>Sonar Sensor</t>
+  </si>
+  <si>
+    <t>PAR Sensor</t>
+  </si>
+  <si>
+    <t>Prototype Controller</t>
+  </si>
+  <si>
+    <t>DIY</t>
+  </si>
+  <si>
+    <t>Soheyl (x1)</t>
+  </si>
+  <si>
+    <t>Soheyl  (x1)</t>
   </si>
 </sst>
 </file>
@@ -735,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8D33D2-063A-4826-9847-26AB4B2A7537}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F34"/>
     </sheetView>
   </sheetViews>
@@ -1310,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB45E8D-C1D9-4D82-89C9-842A5E92CFE0}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" activeCellId="1" sqref="B4 D6:D7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1324,6 +1348,7 @@
     <col min="4" max="4" width="16.88671875" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
     <col min="8" max="8" width="14.21875" customWidth="1"/>
     <col min="9" max="9" width="14.44140625" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" customWidth="1"/>
@@ -1431,6 +1456,82 @@
       </c>
       <c r="I4" s="7">
         <v>45539</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="13">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1</v>
+      </c>
+      <c r="C7" s="15">
+        <v>99.99</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated comprehensive items list
</commit_message>
<xml_diff>
--- a/UVM-NRT-RoS/equipment-records/CIROH_Items_Comprehensive_List.xlsx
+++ b/UVM-NRT-RoS/equipment-records/CIROH_Items_Comprehensive_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CIROH_Repository\CIROH-NextGen-SMS-UVM\UVM-NRT-RoS\equipment-records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3730C9DF-AD33-4914-9F73-C6D1EEB69BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4582B9F-8339-4E79-BC62-A88F8CFB4785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{E103461D-B812-4EE3-B8B5-011B2C0D6DE5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
   <si>
     <t>Item</t>
   </si>
@@ -1337,7 +1337,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1406,6 +1406,9 @@
       <c r="G2" t="s">
         <v>82</v>
       </c>
+      <c r="H2" t="s">
+        <v>89</v>
+      </c>
       <c r="I2" s="7">
         <v>45539</v>
       </c>
@@ -1429,6 +1432,9 @@
       <c r="F3" s="1"/>
       <c r="G3" t="s">
         <v>82</v>
+      </c>
+      <c r="H3" t="s">
+        <v>89</v>
       </c>
       <c r="I3" s="7">
         <v>45539</v>

</xml_diff>

<commit_message>
Updated CIROH_Items_Comprehensive_List. Should now contain all orders from fall 2024
</commit_message>
<xml_diff>
--- a/UVM-NRT-RoS/equipment-records/CIROH_Items_Comprehensive_List.xlsx
+++ b/UVM-NRT-RoS/equipment-records/CIROH_Items_Comprehensive_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CIROH_Repository\CIROH-NextGen-SMS-UVM\UVM-NRT-RoS\equipment-records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4582B9F-8339-4E79-BC62-A88F8CFB4785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FE7DE6-8E6E-47B2-9C04-C0700922C152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{E103461D-B812-4EE3-B8B5-011B2C0D6DE5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="104">
   <si>
     <t>Item</t>
   </si>
@@ -311,6 +311,45 @@
   </si>
   <si>
     <t>Soheyl  (x1)</t>
+  </si>
+  <si>
+    <t>Transducer Contact Microphone</t>
+  </si>
+  <si>
+    <t>Amazon.com: DZS Elec 15PCS 35mm Piezo Disc Transducer Contact Microphone Trigger Sound Sensor with 4 Inches Wires for Acoustic Instrument : Musical Instruments</t>
+  </si>
+  <si>
+    <t>CME0303S3C - Isolated PS</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>Automatic gain controll Microphone</t>
+  </si>
+  <si>
+    <t>Cable (50 feet)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microphone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molex 51021-1000 </t>
+  </si>
+  <si>
+    <t>DigiKey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry pi </t>
+  </si>
+  <si>
+    <t>Fall 2024</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>RockBlock Tranceiver</t>
   </si>
 </sst>
 </file>
@@ -385,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,6 +459,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1334,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB45E8D-C1D9-4D82-89C9-842A5E92CFE0}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1481,6 +1548,9 @@
       <c r="H6" s="13" t="s">
         <v>89</v>
       </c>
+      <c r="I6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -1500,6 +1570,9 @@
       </c>
       <c r="H7" s="13" t="s">
         <v>89</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1519,6 +1592,9 @@
       <c r="H8" s="13" t="s">
         <v>89</v>
       </c>
+      <c r="I8" s="21" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
@@ -1539,12 +1615,177 @@
       <c r="H9" s="13" t="s">
         <v>90</v>
       </c>
+      <c r="I9" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="20">
+        <v>1</v>
+      </c>
+      <c r="C11" s="20">
+        <v>4.99</v>
+      </c>
+      <c r="D11" s="4">
+        <v>4.99</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="17">
+        <v>2</v>
+      </c>
+      <c r="C12" s="20">
+        <v>3.25</v>
+      </c>
+      <c r="D12" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="17">
+        <v>1</v>
+      </c>
+      <c r="C13" s="20">
+        <v>7.95</v>
+      </c>
+      <c r="D13" s="4">
+        <v>7.95</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I16" s="21"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="22">
+        <v>1</v>
+      </c>
+      <c r="C17" s="24">
+        <v>21.99</v>
+      </c>
+      <c r="D17" s="24">
+        <v>21.99</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="22">
+        <v>1</v>
+      </c>
+      <c r="C18" s="24">
+        <v>7.49</v>
+      </c>
+      <c r="D18" s="24">
+        <v>7.49</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="22">
+        <v>5</v>
+      </c>
+      <c r="C19" s="24">
+        <v>0.42</v>
+      </c>
+      <c r="D19" s="24">
+        <v>2.1</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="22">
+        <v>2</v>
+      </c>
+      <c r="C20" s="25">
+        <v>35</v>
+      </c>
+      <c r="D20" s="25">
+        <v>70</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{148F026D-5162-45C8-B353-8F3B64B137EC}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{580BBE86-05CD-4763-BE08-5C3BA1726166}"/>
     <hyperlink ref="E4" r:id="rId3" display="https://www.envirodiy.org/product/envirodiy-mayfly-data-logger/" xr:uid="{02D1B82F-BFD8-4855-BBB5-F0F6CF697B07}"/>
+    <hyperlink ref="E12" r:id="rId4" xr:uid="{75126B7F-8802-415D-9A08-589CA8918A30}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{A66DB734-2AED-4C4D-A8B0-9C7BD48E39E5}"/>
+    <hyperlink ref="E11" r:id="rId6" display="https://www.amazon.com/DZS-Elec-Transducer-Microphone-Instrument/dp/B084KHH7B6/ref=sr_1_19?dib=eyJ2IjoiMSJ9.-PibDNlinRz79bIpdumGJKLNDqgwo8MJ5Yur3e9XNYKUOlqtMaPkT5RbNL1UTHdk9PlMjYh8k938pDwecAJ3MBVB5GgJp0aDSe5PK_QLgmFmKujHDdR2CkbwuTbrQngjvjEtKLfrqUjdOWQv28gJyphTne3z90EQrXzwTVcDgEgUVL52XbIaM1IbMUQgsKnKgYSKWdKSTIkeM-uaM6fUkM3cPWOA0B2ba7SIURtCjegOvJMqLDOWVxTC8Gz3ygrqHVCl8lisiaulh38ciug__mY2EYUkTgSYbwo3FhV8imc.8H3H4oIOGSwKLzykTkDj1mJYWcn7OKWwjFTXtMVt8R8&amp;dib_tag=se&amp;keywords=contact%2Bmicrophone&amp;qid=1726071396&amp;sr=8-19&amp;th=1" xr:uid="{14BE9BF3-6D39-464E-9058-565F5585CDB4}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{30824719-4DBB-43D7-893D-640B435A6593}"/>
+    <hyperlink ref="E18" r:id="rId8" xr:uid="{1A3D08D6-4DDB-45EB-938A-58F1D58E7958}"/>
+    <hyperlink ref="E19" r:id="rId9" xr:uid="{F89C2761-C318-CD44-BD3D-246096CD0D60}"/>
+    <hyperlink ref="E20" r:id="rId10" xr:uid="{5B5EC256-2F51-48BE-80CA-DC72A6652EA0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>